<commit_message>
Continuation of exec summary
</commit_message>
<xml_diff>
--- a/Comparison/Word count.xlsx
+++ b/Comparison/Word count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\MSc-Project\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A48279-BC9F-4EBE-8643-085C4EF74D7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E62EFAE-2CD7-4323-A5AC-F6A8C2FC206C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5A438F4-76E6-4718-8920-804AE3072837}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F96CE2-C24A-4465-B4B6-D81433725DCD}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +818,20 @@
         <v>19792</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43696</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.51944444444444449</v>
+      </c>
+      <c r="C31">
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>19928</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Intro and summary for chapt 1
</commit_message>
<xml_diff>
--- a/Comparison/Word count.xlsx
+++ b/Comparison/Word count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\MSc-Project\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8503F-89B0-473B-867D-F0BB6D5376F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D01652-A302-44B4-8585-C89650ECEC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5A438F4-76E6-4718-8920-804AE3072837}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F96CE2-C24A-4465-B4B6-D81433725DCD}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,6 +932,20 @@
       </c>
       <c r="D38">
         <v>20644</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="C39">
+        <v>74</v>
+      </c>
+      <c r="D39">
+        <v>21139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lit review intro changed
</commit_message>
<xml_diff>
--- a/Comparison/Word count.xlsx
+++ b/Comparison/Word count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\MSc-Project\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D01652-A302-44B4-8585-C89650ECEC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E870E-CD54-4BEF-BBF1-E865E4DEE4CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5A438F4-76E6-4718-8920-804AE3072837}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F96CE2-C24A-4465-B4B6-D81433725DCD}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,6 +946,34 @@
       </c>
       <c r="D39">
         <v>21139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C40">
+        <v>72</v>
+      </c>
+      <c r="D40">
+        <v>21484</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="C41">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>21449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intro and summary for implementation
</commit_message>
<xml_diff>
--- a/Comparison/Word count.xlsx
+++ b/Comparison/Word count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\MSc-Project\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E870E-CD54-4BEF-BBF1-E865E4DEE4CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6524FB56-DE44-4136-9A8C-D8E292FCD11A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5A438F4-76E6-4718-8920-804AE3072837}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F96CE2-C24A-4465-B4B6-D81433725DCD}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +850,7 @@
         <v>20037</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43696</v>
       </c>
@@ -864,7 +864,7 @@
         <v>20382</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43696</v>
       </c>
@@ -878,7 +878,7 @@
         <v>20337</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43696</v>
       </c>
@@ -892,7 +892,7 @@
         <v>20325</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43696</v>
       </c>
@@ -906,7 +906,7 @@
         <v>20579</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43696</v>
       </c>
@@ -920,7 +920,7 @@
         <v>20585</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43696</v>
       </c>
@@ -934,7 +934,7 @@
         <v>20644</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43697</v>
       </c>
@@ -948,7 +948,7 @@
         <v>21139</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43697</v>
       </c>
@@ -962,7 +962,7 @@
         <v>21484</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43697</v>
       </c>
@@ -974,6 +974,51 @@
       </c>
       <c r="D41">
         <v>21449</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="C42">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>21888</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C43">
+        <v>72</v>
+      </c>
+      <c r="D43">
+        <v>21920</v>
+      </c>
+      <c r="E43">
+        <v>17413</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C44">
+        <v>72</v>
+      </c>
+      <c r="D44">
+        <v>22261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more content to comparisons
</commit_message>
<xml_diff>
--- a/Comparison/Word count.xlsx
+++ b/Comparison/Word count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\MSc-Project\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61588421-005D-48A5-8891-45BC60C70BC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38485F6A-89AF-44AF-A77C-D422AE4D4603}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5A438F4-76E6-4718-8920-804AE3072837}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F96CE2-C24A-4465-B4B6-D81433725DCD}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,6 +1053,48 @@
       </c>
       <c r="E46">
         <v>17891</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43698</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C47">
+        <v>74</v>
+      </c>
+      <c r="D47">
+        <v>22409</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43698</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="C48">
+        <v>74</v>
+      </c>
+      <c r="D48">
+        <v>22670</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43698</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="C49">
+        <v>74</v>
+      </c>
+      <c r="D49">
+        <v>22392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through control-flow tracing
</commit_message>
<xml_diff>
--- a/Comparison/Word count.xlsx
+++ b/Comparison/Word count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\MSc-Project\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD7DF5C-C7CA-4208-A661-05D97611C550}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A8F999-0E55-4FEE-ADE7-BA4E36141B59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5A438F4-76E6-4718-8920-804AE3072837}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F96CE2-C24A-4465-B4B6-D81433725DCD}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1109,20 @@
       </c>
       <c r="D50">
         <v>22485</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43698</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="C51">
+        <v>74</v>
+      </c>
+      <c r="D51">
+        <v>22658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>